<commit_message>
Update Payto in rfd_prnt
</commit_message>
<xml_diff>
--- a/AOQ Five.xlsx
+++ b/AOQ Five.xlsx
@@ -15,31 +15,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
   <si>
     <t>ABSTRACT OF QUOTATION</t>
   </si>
   <si>
-    <t xml:space="preserve">Department: Accounting Department
+    <t xml:space="preserve">Department: Auxiliary
 </t>
   </si>
   <si>
-    <t>Date: June 3, 2019</t>
-  </si>
-  <si>
-    <t>Purpose: 23 Additional CCTV Requirements at CENPRI Site</t>
-  </si>
-  <si>
-    <t>PR#: PR1010101</t>
+    <t>Date: June 7, 2019</t>
+  </si>
+  <si>
+    <t>Purpose: 40MVA Power Transformer Secondary Bus Framing/Support</t>
+  </si>
+  <si>
+    <t>PR#: PR4567</t>
   </si>
   <si>
     <t>Enduse: 1.5 MVA Station Transformer DG4 &amp; DG5 Generator Wi</t>
   </si>
   <si>
-    <t>Date Needed: May 2, 2018</t>
+    <t>Date Needed: May 6, 2018</t>
   </si>
   <si>
     <t>Requested By: Accounting Department</t>
+  </si>
+  <si>
+    <t>Bacolod Visayan Lumber
+433-8888</t>
+  </si>
+  <si>
+    <t>Ablao Enterprises
+461-0376</t>
+  </si>
+  <si>
+    <t>A-one Industrial Sales
+Ms. Miles
+435-7383; 432-0652; 476-1127</t>
+  </si>
+  <si>
+    <t>Visayan Construction Supply
+434-7277 / 434-7278</t>
   </si>
   <si>
     <t>Ava Construction Supply
@@ -47,19 +64,6 @@
 434-1822; 433-0263; 435-1901; 708-3757</t>
   </si>
   <si>
-    <t>Ablao Enterprises
-461-0376</t>
-  </si>
-  <si>
-    <t>A-one Industrial Sales
-Ms. Miles
-435-7383; 432-0652; 476-1127</t>
-  </si>
-  <si>
-    <t>Visayan Construction Supply
-434-7277 / 434-7278</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
@@ -87,40 +91,82 @@
     <t>Grinding Disc</t>
   </si>
   <si>
-    <t>asdasdasd, Grinding Disc</t>
-  </si>
-  <si>
-    <t>bebebbee, Grinding Disc</t>
-  </si>
-  <si>
-    <t>Brandx, Grinding Disc</t>
-  </si>
-  <si>
-    <t>Brandf, Grinding Disc</t>
-  </si>
-  <si>
-    <t>Brandssss, Grinding Disc</t>
+    <t>brandoffer3, Grinding Disc</t>
+  </si>
+  <si>
+    <t>comment1</t>
+  </si>
+  <si>
+    <t>brandoffer5, Grinding Disc</t>
+  </si>
+  <si>
+    <t>comment2</t>
+  </si>
+  <si>
+    <t>brandy, Grinding Disc</t>
+  </si>
+  <si>
+    <t>comment3</t>
+  </si>
+  <si>
+    <t>offer2, Grinding Disc</t>
+  </si>
+  <si>
+    <t>comment4</t>
   </si>
   <si>
     <t>Cutting Disc</t>
   </si>
   <si>
-    <t>asdasd, Cutting Disc</t>
-  </si>
-  <si>
-    <t>bababab, Cutting Disc</t>
-  </si>
-  <si>
-    <t>Brands, Cutting Disc</t>
-  </si>
-  <si>
-    <t>Brandy, Cutting Disc</t>
-  </si>
-  <si>
-    <t>Brand3, Cutting Disc</t>
-  </si>
-  <si>
-    <t>Brandl, Cutting Disc</t>
+    <t>brandoffer2, Cutting Disc</t>
+  </si>
+  <si>
+    <t>comment5</t>
+  </si>
+  <si>
+    <t>brandoffer4, Cutting Disc</t>
+  </si>
+  <si>
+    <t>comment6</t>
+  </si>
+  <si>
+    <t>brands, Cutting Disc</t>
+  </si>
+  <si>
+    <t>comment7</t>
+  </si>
+  <si>
+    <t>brand1, Cutting Disc</t>
+  </si>
+  <si>
+    <t>comment8</t>
+  </si>
+  <si>
+    <t>offer1, Cutting Disc</t>
+  </si>
+  <si>
+    <t>comment9</t>
+  </si>
+  <si>
+    <t>Plywood</t>
+  </si>
+  <si>
+    <t>brandoffer1, Plywood</t>
+  </si>
+  <si>
+    <t>Brandx, Plywood</t>
+  </si>
+  <si>
+    <t>comment10</t>
+  </si>
+  <si>
+    <t>brandsss, Plywood</t>
+  </si>
+  <si>
+    <t>comment11</t>
+  </si>
+  <si>
+    <t>brandyy, Plywood</t>
   </si>
   <si>
     <t>a. Price Validity</t>
@@ -132,7 +178,7 @@
     <t>c. Date of Delivery</t>
   </si>
   <si>
-    <t>May 31, 2019</t>
+    <t>June 7, 2019</t>
   </si>
   <si>
     <t>d. Items Warranty</t>
@@ -156,7 +202,7 @@
     <t>Accounting Department</t>
   </si>
   <si>
-    <t>Carlito Alevio</t>
+    <t>Caesariane Jo</t>
   </si>
   <si>
     <t>Celina Marie Grabillo</t>
@@ -208,13 +254,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFf4e542"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFf4e542"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -263,6 +309,12 @@
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="4" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="4" fillId="0" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
@@ -277,12 +329,6 @@
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="4" fillId="3" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -592,7 +638,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:X25"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A8" sqref="A8"/>
@@ -602,25 +648,25 @@
   <cols>
     <col min="1" max="1" width="2.285156" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="16.424561" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="69.554443" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="74.267578" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="26.993408" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="29.421387" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="28.135986" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="31.706543" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="6.998291" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="25.85083" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="10.568848" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="25.85083" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="8.140869" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="11.711426" bestFit="true" customWidth="true" style="0"/>
     <col min="17" max="17" width="24.708252" bestFit="true" customWidth="true" style="0"/>
     <col min="18" max="18" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="29.421387" bestFit="true" customWidth="true" style="0"/>
-    <col min="22" max="22" width="6.998291" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="25.85083" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="10.568848" bestFit="true" customWidth="true" style="0"/>
     <col min="24" max="24" width="10.568848" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
@@ -660,109 +706,109 @@
       </c>
     </row>
     <row r="7" spans="1:24">
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="8" t="s">
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="8" t="s">
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="8" t="s">
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="R7" s="10"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="V7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="9"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="11"/>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="D8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="F8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="G8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="7" t="s">
+      <c r="H8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="J8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="K8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="N8" s="7" t="s">
+      <c r="L8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="N8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="O8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="R8" s="7" t="s">
+      <c r="P8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="S8" s="7" t="s">
+      <c r="R8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="T8" s="7" t="s">
+      <c r="S8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="U8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="V8" s="7" t="s">
+      <c r="T8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="U8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="W8" s="7" t="s">
+      <c r="V8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="X8" s="7" t="s">
+      <c r="W8" s="9" t="s">
         <v>19</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -770,147 +816,191 @@
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4">
         <v>10</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9" s="6">
-        <v>70</v>
-      </c>
-      <c r="G9" s="6">
-        <v>700</v>
-      </c>
-      <c r="H9" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="G9" s="7">
+        <v>300</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="I9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="6">
-        <v>10</v>
-      </c>
-      <c r="K9" s="11">
+        <v>24</v>
+      </c>
+      <c r="J9" s="8">
+        <v>50</v>
+      </c>
+      <c r="K9" s="8">
+        <v>500</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" s="8">
         <v>100</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="6">
-        <v>200</v>
-      </c>
-      <c r="O9" s="6">
-        <v>2000</v>
-      </c>
-      <c r="P9" s="3"/>
+      <c r="O9" s="8">
+        <v>1000</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="Q9" s="3"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
       <c r="T9" s="3"/>
       <c r="U9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="V9" s="6">
-        <v>60</v>
-      </c>
-      <c r="W9" s="6">
-        <v>600</v>
-      </c>
-      <c r="X9" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="V9" s="8">
+        <v>170</v>
+      </c>
+      <c r="W9" s="8">
+        <v>1700</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="3">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="4">
+        <v>50</v>
+      </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="3"/>
+      <c r="E10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="6">
+        <v>20</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1000</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="8">
+        <v>40</v>
+      </c>
+      <c r="K10" s="7">
+        <v>2000</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" s="8">
+        <v>200</v>
+      </c>
+      <c r="O10" s="8">
+        <v>10000</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R10" s="8">
+        <v>150</v>
+      </c>
+      <c r="S10" s="8">
+        <v>7500</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="U10" s="5" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="V10" s="6">
-        <v>0</v>
-      </c>
-      <c r="W10" s="6"/>
-      <c r="X10" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="W10" s="8">
+        <v>1000</v>
+      </c>
+      <c r="X10" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:24">
       <c r="A11" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C11" s="4">
         <v>10</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="5" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="F11" s="6">
-        <v>60</v>
-      </c>
-      <c r="G11" s="6">
-        <v>600</v>
-      </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="12">
-        <v>50</v>
-      </c>
-      <c r="K11" s="11">
-        <v>500</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G11" s="8">
+        <v>100</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
       <c r="L11" s="3"/>
       <c r="M11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N11" s="6">
+        <v>43</v>
+      </c>
+      <c r="N11" s="8">
+        <v>50</v>
+      </c>
+      <c r="O11" s="7">
+        <v>500</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="R11" s="8">
+        <v>30</v>
+      </c>
+      <c r="S11" s="8">
         <v>300</v>
       </c>
-      <c r="O11" s="6">
-        <v>3000</v>
-      </c>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="R11" s="6">
-        <v>500</v>
-      </c>
-      <c r="S11" s="6">
-        <v>5000</v>
-      </c>
-      <c r="T11" s="3"/>
-      <c r="U11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="V11" s="12">
-        <v>50</v>
-      </c>
-      <c r="W11" s="6">
-        <v>500</v>
-      </c>
+      <c r="T11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="U11" s="3"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
       <c r="X11" s="3"/>
     </row>
     <row r="12" spans="1:24">
@@ -919,62 +1009,87 @@
       <c r="C12" s="4"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
       <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="V12" s="6">
-        <v>80</v>
-      </c>
-      <c r="W12" s="6">
-        <v>800</v>
-      </c>
+      <c r="Q12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="R12" s="8">
+        <v>100</v>
+      </c>
+      <c r="S12" s="8">
+        <v>1000</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="U12" s="3"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
       <c r="X12" s="3"/>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="Q13" s="13">
+        <v>1</v>
+      </c>
+      <c r="R13" s="14"/>
+      <c r="S13" s="14"/>
+      <c r="U13" s="13">
+        <v>2</v>
+      </c>
+      <c r="V13" s="14"/>
+      <c r="W13" s="14"/>
     </row>
     <row r="15" spans="1:24">
       <c r="C15" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
-      <c r="H15"/>
       <c r="I15" s="13"/>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
-      <c r="M15" s="13">
-        <v>1</v>
-      </c>
+      <c r="L15"/>
+      <c r="M15" s="13"/>
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
       <c r="Q15" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R15" s="14"/>
       <c r="S15" s="14"/>
       <c r="U15" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V15" s="14"/>
       <c r="W15" s="14"/>
     </row>
     <row r="17" spans="1:24">
       <c r="C17" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="14"/>
@@ -982,26 +1097,24 @@
       <c r="I17" s="13"/>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
-      <c r="L17"/>
-      <c r="M17" s="13">
-        <v>1</v>
-      </c>
+      <c r="M17" s="13"/>
       <c r="N17" s="14"/>
       <c r="O17" s="14"/>
-      <c r="Q17" s="13">
-        <v>2</v>
+      <c r="P17"/>
+      <c r="Q17" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="R17" s="14"/>
       <c r="S17" s="14"/>
-      <c r="U17" s="13">
-        <v>3</v>
+      <c r="U17" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="V17" s="14"/>
       <c r="W17" s="14"/>
     </row>
     <row r="19" spans="1:24">
       <c r="C19" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
@@ -1009,75 +1122,46 @@
       <c r="I19" s="13"/>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
-      <c r="M19" s="13" t="s">
-        <v>36</v>
-      </c>
+      <c r="M19" s="13"/>
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
-      <c r="P19"/>
-      <c r="Q19" s="13" t="s">
-        <v>36</v>
+      <c r="Q19" s="13">
+        <v>2</v>
       </c>
       <c r="R19" s="14"/>
       <c r="S19" s="14"/>
-      <c r="U19" s="13" t="s">
-        <v>36</v>
+      <c r="U19" s="13">
+        <v>22</v>
       </c>
       <c r="V19" s="14"/>
       <c r="W19" s="14"/>
     </row>
     <row r="21" spans="1:24">
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="M21" s="13">
-        <v>1</v>
-      </c>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="Q21" s="13">
-        <v>2</v>
-      </c>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="U21" s="13">
-        <v>3</v>
-      </c>
-      <c r="V21" s="14"/>
-      <c r="W21" s="14"/>
+      <c r="E21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="23" spans="1:24">
-      <c r="E23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24">
-      <c r="E25" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="I25" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="K25" s="15" t="s">
-        <v>45</v>
+      <c r="E23" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1089,9 +1173,9 @@
     <mergeCell ref="M7:P7"/>
     <mergeCell ref="Q7:T7"/>
     <mergeCell ref="U7:X7"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="M17:P17"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>